<commit_message>
added mil personnel estimates
</commit_message>
<xml_diff>
--- a/Data files/Raw data files/185674.xlsx
+++ b/Data files/Raw data files/185674.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmyballesteros/R/conflict-relapse/Data files/Raw data files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92994DCE-6AA9-E043-949F-8104F914FFA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1371633-49F7-044E-86C4-AC4E9D06EEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17420" yWindow="780" windowWidth="17140" windowHeight="20880" xr2:uid="{210E191D-1934-E14E-8B96-C96F93DDA747}"/>
   </bookViews>
@@ -796,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -807,36 +807,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -853,11 +823,40 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1195,8 +1194,8 @@
   <dimension ref="A1:W1919"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <pane ySplit="5" topLeftCell="A286" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B316" sqref="B316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1227,173 +1226,173 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
     </row>
     <row r="4" spans="1:23" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="15" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="18" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="15" t="s">
+      <c r="K4" s="18"/>
+      <c r="L4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="17"/>
-      <c r="N4" s="18" t="s">
+      <c r="M4" s="27"/>
+      <c r="N4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="18" t="s">
+      <c r="O4" s="18"/>
+      <c r="P4" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="18" t="s">
+      <c r="Q4" s="18"/>
+      <c r="R4" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="S4" s="19"/>
-      <c r="T4" s="18" t="s">
+      <c r="S4" s="18"/>
+      <c r="T4" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="U4" s="19"/>
-      <c r="V4" s="18" t="s">
+      <c r="U4" s="18"/>
+      <c r="V4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="W4" s="19"/>
+      <c r="W4" s="18"/>
     </row>
     <row r="5" spans="1:23" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="22" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="20" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="22" t="s">
+      <c r="G5" s="11"/>
+      <c r="H5" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="23" t="s">
+      <c r="I5" s="11"/>
+      <c r="J5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="24"/>
-      <c r="L5" s="23" t="s">
+      <c r="K5" s="14"/>
+      <c r="L5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="24"/>
-      <c r="N5" s="22" t="s">
+      <c r="M5" s="14"/>
+      <c r="N5" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="O5" s="24"/>
-      <c r="P5" s="22" t="s">
+      <c r="O5" s="14"/>
+      <c r="P5" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="22" t="s">
+      <c r="Q5" s="14"/>
+      <c r="R5" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="S5" s="24"/>
-      <c r="T5" s="22" t="s">
+      <c r="S5" s="14"/>
+      <c r="T5" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="U5" s="25"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
@@ -1518,34 +1517,34 @@
       <c r="A10" s="6">
         <v>1966</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="1">
         <v>14.42</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="1">
         <v>14.02</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="1">
         <v>891.1</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="1">
         <v>866.2</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="1">
         <v>1.62</v>
       </c>
-      <c r="L10" s="28">
+      <c r="L10" s="1">
         <v>15.6</v>
       </c>
-      <c r="N10" s="28">
+      <c r="N10" s="1">
         <v>0.9</v>
       </c>
-      <c r="P10" s="28">
+      <c r="P10" s="1">
         <v>56</v>
       </c>
-      <c r="R10" s="28">
+      <c r="R10" s="1">
         <v>97</v>
       </c>
-      <c r="T10" s="28">
+      <c r="T10" s="1">
         <v>145</v>
       </c>
       <c r="V10" s="1">
@@ -1556,34 +1555,34 @@
       <c r="A11" s="6">
         <v>1967</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="1">
         <v>15.58</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="1">
         <v>15.02</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="1">
         <v>918.2</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="1">
         <v>885.4</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="1">
         <v>1.7</v>
       </c>
-      <c r="L11" s="28">
+      <c r="L11" s="1">
         <v>15.9</v>
       </c>
-      <c r="N11" s="28">
+      <c r="N11" s="1">
         <v>0.94</v>
       </c>
-      <c r="P11" s="28">
+      <c r="P11" s="1">
         <v>56</v>
       </c>
-      <c r="R11" s="28">
+      <c r="R11" s="1">
         <v>95</v>
       </c>
-      <c r="T11" s="28">
+      <c r="T11" s="1">
         <v>158</v>
       </c>
       <c r="V11" s="1">
@@ -1594,34 +1593,34 @@
       <c r="A12" s="6">
         <v>1968</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="1">
         <v>17.63</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="1">
         <v>16.5</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="1">
         <v>974.1</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="1">
         <v>912.1</v>
       </c>
-      <c r="J12" s="28">
+      <c r="J12" s="1">
         <v>1.81</v>
       </c>
-      <c r="L12" s="28">
+      <c r="L12" s="1">
         <v>16.3</v>
       </c>
-      <c r="N12" s="28">
+      <c r="N12" s="1">
         <v>1.01</v>
       </c>
-      <c r="P12" s="28">
+      <c r="P12" s="1">
         <v>56</v>
       </c>
-      <c r="R12" s="28">
+      <c r="R12" s="1">
         <v>89</v>
       </c>
-      <c r="T12" s="28">
+      <c r="T12" s="1">
         <v>185</v>
       </c>
       <c r="V12" s="1">
@@ -1632,34 +1631,34 @@
       <c r="A13" s="6">
         <v>1969</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="1">
         <v>17.8</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="1">
         <v>17.03</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="1">
         <v>992</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="1">
         <v>949</v>
       </c>
-      <c r="J13" s="28">
+      <c r="J13" s="1">
         <v>1.79</v>
       </c>
-      <c r="L13" s="28">
+      <c r="L13" s="1">
         <v>16.7</v>
       </c>
-      <c r="N13" s="28">
+      <c r="N13" s="1">
         <v>1.02</v>
       </c>
-      <c r="P13" s="28">
+      <c r="P13" s="1">
         <v>57</v>
       </c>
-      <c r="R13" s="28">
+      <c r="R13" s="1">
         <v>89</v>
       </c>
-      <c r="T13" s="28">
+      <c r="T13" s="1">
         <v>191</v>
       </c>
       <c r="V13" s="1">
@@ -1670,34 +1669,34 @@
       <c r="A14" s="6">
         <v>1970</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="1">
         <v>16.73</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="1">
         <v>17.34</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="1">
         <v>941.4</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="1">
         <v>975.7</v>
       </c>
-      <c r="J14" s="28">
+      <c r="J14" s="1">
         <v>1.78</v>
       </c>
-      <c r="L14" s="28">
+      <c r="L14" s="1">
         <v>17.100000000000001</v>
       </c>
-      <c r="N14" s="28">
+      <c r="N14" s="1">
         <v>1.01</v>
       </c>
-      <c r="P14" s="28">
+      <c r="P14" s="1">
         <v>57</v>
       </c>
-      <c r="R14" s="28">
+      <c r="R14" s="1">
         <v>91</v>
       </c>
-      <c r="T14" s="28">
+      <c r="T14" s="1">
         <v>191</v>
       </c>
       <c r="V14" s="1">
@@ -1708,34 +1707,34 @@
       <c r="A15" s="6">
         <v>1971</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="1">
         <v>15.6</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D15" s="1">
         <v>17.07</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F15" s="1">
         <v>913.8</v>
       </c>
-      <c r="H15" s="28">
+      <c r="H15" s="1">
         <v>999.9</v>
       </c>
-      <c r="J15" s="28">
+      <c r="J15" s="1">
         <v>1.71</v>
       </c>
-      <c r="L15" s="28">
+      <c r="L15" s="1">
         <v>17.5</v>
       </c>
-      <c r="N15" s="28">
+      <c r="N15" s="1">
         <v>0.98</v>
       </c>
-      <c r="P15" s="28">
+      <c r="P15" s="1">
         <v>57</v>
       </c>
-      <c r="R15" s="28">
+      <c r="R15" s="1">
         <v>91</v>
       </c>
-      <c r="T15" s="28">
+      <c r="T15" s="1">
         <v>188</v>
       </c>
       <c r="V15" s="1">
@@ -1746,34 +1745,34 @@
       <c r="A16" s="6">
         <v>1972</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="1">
         <v>17.05</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="1">
         <v>17.05</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="1">
         <v>1027.8</v>
       </c>
-      <c r="H16" s="28">
+      <c r="H16" s="1">
         <v>1027.8</v>
       </c>
-      <c r="J16" s="28">
+      <c r="J16" s="1">
         <v>1.66</v>
       </c>
-      <c r="L16" s="28">
+      <c r="L16" s="1">
         <v>17.899999999999999</v>
       </c>
-      <c r="N16" s="28">
+      <c r="N16" s="1">
         <v>0.95</v>
       </c>
-      <c r="P16" s="28">
+      <c r="P16" s="1">
         <v>57</v>
       </c>
-      <c r="R16" s="28">
+      <c r="R16" s="1">
         <v>91</v>
       </c>
-      <c r="T16" s="28">
+      <c r="T16" s="1">
         <v>187</v>
       </c>
       <c r="V16" s="1">
@@ -1784,31 +1783,31 @@
       <c r="A17" s="6">
         <v>1973</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="1">
         <v>21.99</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="1" t="s">
         <v>145</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="H17" s="28">
+      <c r="H17" s="1">
         <v>1056.5999999999999</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="L17" s="28">
+      <c r="L17" s="1">
         <v>18.3</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="P17" s="28">
+      <c r="P17" s="1">
         <v>58</v>
       </c>
-      <c r="R17" s="28">
+      <c r="R17" s="1">
         <v>91</v>
       </c>
       <c r="T17" s="1" t="s">
@@ -1822,25 +1821,25 @@
       <c r="A18" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D18" s="1">
         <v>7</v>
       </c>
-      <c r="H18" s="28">
+      <c r="H18" s="1">
         <v>2.7</v>
       </c>
       <c r="J18" s="1">
         <v>4.2</v>
       </c>
-      <c r="L18" s="28">
+      <c r="L18" s="1">
         <v>2.2999999999999998</v>
       </c>
       <c r="N18" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="P18" s="28">
+      <c r="P18" s="1">
         <v>0.4</v>
       </c>
-      <c r="R18" s="28">
+      <c r="R18" s="1">
         <v>-1.9</v>
       </c>
       <c r="T18" s="1">
@@ -11412,7 +11411,7 @@
         <v>1972</v>
       </c>
       <c r="B313" s="1">
-        <v>145000</v>
+        <v>14500</v>
       </c>
       <c r="D313" s="1">
         <v>14500</v>
@@ -11450,7 +11449,7 @@
         <v>1973</v>
       </c>
       <c r="B314" s="1">
-        <v>145000</v>
+        <v>15000</v>
       </c>
       <c r="D314" s="1">
         <v>14200</v>
@@ -11487,9 +11486,6 @@
       <c r="A315" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="B315" s="1">
-        <v>15000</v>
-      </c>
       <c r="D315" s="1">
         <v>8</v>
       </c>
@@ -13357,7 +13353,7 @@
       <c r="L371" s="1">
         <v>3.1</v>
       </c>
-      <c r="N371" s="27" t="s">
+      <c r="N371" s="16" t="s">
         <v>149</v>
       </c>
       <c r="P371" s="1">
@@ -13366,7 +13362,7 @@
       <c r="R371" s="1">
         <v>0</v>
       </c>
-      <c r="T371" s="27" t="s">
+      <c r="T371" s="16" t="s">
         <v>149</v>
       </c>
       <c r="V371" s="1">

</xml_diff>